<commit_message>
avoid test data-clash with prod db
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1605.8.metagenome.xlsx
+++ b/tests/fixtures/orderforms/1605.8.metagenome.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0914A5-54D4-0442-ADFB-0A3521111C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="2860" windowWidth="33680" windowHeight="21420" tabRatio="283" activeTab="1"/>
+    <workbookView xWindow="2400" yWindow="760" windowWidth="33600" windowHeight="20540" tabRatio="283" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="4" r:id="rId1"/>
     <sheet name="order form" sheetId="1" r:id="rId2"/>
     <sheet name="Drop down list" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1369,76 +1375,76 @@
     <t>Bug fix related to Document header</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>s3</t>
-  </si>
-  <si>
     <t>EB-buffer</t>
   </si>
   <si>
-    <t>s4</t>
-  </si>
-  <si>
-    <t>s5</t>
-  </si>
-  <si>
-    <t>s6</t>
-  </si>
-  <si>
-    <t>s7</t>
-  </si>
-  <si>
-    <t>s8</t>
-  </si>
-  <si>
-    <t>s9</t>
-  </si>
-  <si>
-    <t>s10</t>
-  </si>
-  <si>
-    <t>s11</t>
-  </si>
-  <si>
-    <t>s12</t>
-  </si>
-  <si>
-    <t>s13</t>
-  </si>
-  <si>
-    <t>s14</t>
-  </si>
-  <si>
-    <t>s15</t>
-  </si>
-  <si>
-    <t>s16</t>
-  </si>
-  <si>
-    <t>s17</t>
-  </si>
-  <si>
-    <t>s18</t>
-  </si>
-  <si>
-    <t>s19</t>
-  </si>
-  <si>
     <t>plate1</t>
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>sample6</t>
+  </si>
+  <si>
+    <t>sample7</t>
+  </si>
+  <si>
+    <t>sample8</t>
+  </si>
+  <si>
+    <t>sample9</t>
+  </si>
+  <si>
+    <t>sample10</t>
+  </si>
+  <si>
+    <t>sample11</t>
+  </si>
+  <si>
+    <t>sample12</t>
+  </si>
+  <si>
+    <t>sample13</t>
+  </si>
+  <si>
+    <t>sample14</t>
+  </si>
+  <si>
+    <t>sample15</t>
+  </si>
+  <si>
+    <t>sample16</t>
+  </si>
+  <si>
+    <t>sample17</t>
+  </si>
+  <si>
+    <t>sample18</t>
+  </si>
+  <si>
+    <t>sample19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -2428,6 +2434,16 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2443,261 +2459,251 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="134" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="244">
-    <cellStyle name="Excel Built-in Normal" xfId="45"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8"/>
-    <cellStyle name="Input" xfId="241" builtinId="20"/>
+    <cellStyle name="Excel Built-in Normal" xfId="45" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="134" builtinId="8"/>
+    <cellStyle name="Indata" xfId="241" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2801,7 +2807,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2476074-2F91-D547-AE5A-5443F535D2A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2476074-2F91-D547-AE5A-5443F535D2A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2850,7 +2856,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3185,7 +3191,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3229,7 +3235,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3250,14 +3256,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="88" style="76" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="76" customWidth="1"/>
@@ -3265,7 +3271,7 @@
     <col min="4" max="16384" width="10.83203125" style="76"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14">
+    <row r="1" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A1" s="75"/>
       <c r="B1" s="75" t="s">
         <v>23</v>
@@ -3276,14 +3282,14 @@
       <c r="D1" s="12"/>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="77"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="78"/>
       <c r="B3" s="78" t="s">
         <v>24</v>
@@ -3296,7 +3302,7 @@
       </c>
       <c r="E3" s="80"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="78"/>
       <c r="B4" s="78" t="s">
         <v>25</v>
@@ -3311,226 +3317,226 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18">
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="82" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="83" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28" customHeight="1">
+    <row r="16" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="99" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="21" customHeight="1">
+    <row r="17" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="99"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="85" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="24">
+    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="84" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60">
+    <row r="20" spans="1:5" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="84" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="36">
+    <row r="21" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A21" s="84" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="85" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="86" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="36">
+    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A25" s="87" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24">
+    <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A26" s="88" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="24">
+    <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="88" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="24">
+    <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="88" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="24">
+    <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="88" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="48">
+    <row r="30" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A30" s="87" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="34" customHeight="1">
+    <row r="31" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="89" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" customHeight="1">
+    <row r="32" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="89" t="s">
         <v>308</v>
       </c>
       <c r="C32" s="84"/>
       <c r="E32" s="84"/>
     </row>
-    <row r="33" spans="1:5" ht="24">
+    <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A33" s="88" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="24">
+    <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A34" s="87" t="s">
         <v>303</v>
       </c>
       <c r="C34" s="84"/>
       <c r="E34" s="84"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35"/>
       <c r="C35" s="84"/>
       <c r="E35" s="84"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="86" t="s">
         <v>295</v>
       </c>
       <c r="E36" s="84"/>
     </row>
-    <row r="37" spans="1:5" ht="27" customHeight="1">
+    <row r="37" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="87" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="24" customHeight="1">
+    <row r="38" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="90" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="24" customHeight="1"/>
-    <row r="40" spans="1:5">
+    <row r="39" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="86" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="24">
+    <row r="41" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="87" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24">
+    <row r="42" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="87" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="90" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="84"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="84"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="84"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="91"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="84"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="84"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="84"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="84"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" s="84"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="84"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" s="84"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="84"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="84"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="84"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="84"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="84"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="84"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="84"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="84"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="84"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="84"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="84"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" s="84"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="84"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1"/>
+    <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3544,17 +3550,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S150"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21:Q21"/>
+      <selection activeCell="A21" sqref="A21:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="3" width="14.33203125" style="2" customWidth="1"/>
@@ -3576,7 +3582,7 @@
     <col min="19" max="16384" width="13.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" hidden="1">
+    <row r="1" spans="1:19" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1" s="75" t="s">
         <v>23</v>
       </c>
@@ -3601,7 +3607,7 @@
       <c r="R1" s="38"/>
       <c r="S1" s="38"/>
     </row>
-    <row r="2" spans="1:19" ht="16" hidden="1">
+    <row r="2" spans="1:19" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -3622,7 +3628,7 @@
       <c r="R2" s="38"/>
       <c r="S2" s="38"/>
     </row>
-    <row r="3" spans="1:19" ht="14" hidden="1">
+    <row r="3" spans="1:19" ht="14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="61"/>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
@@ -3643,7 +3649,7 @@
       <c r="R3" s="38"/>
       <c r="S3" s="38"/>
     </row>
-    <row r="4" spans="1:19" ht="14" hidden="1">
+    <row r="4" spans="1:19" ht="14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="61"/>
       <c r="B4" s="61"/>
       <c r="C4" s="61"/>
@@ -3664,7 +3670,7 @@
       <c r="R4" s="38"/>
       <c r="S4" s="38"/>
     </row>
-    <row r="5" spans="1:19" ht="16" hidden="1">
+    <row r="5" spans="1:19" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -3685,7 +3691,7 @@
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
     </row>
-    <row r="6" spans="1:19" ht="16" hidden="1">
+    <row r="6" spans="1:19" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -3706,7 +3712,7 @@
       <c r="R6" s="38"/>
       <c r="S6" s="38"/>
     </row>
-    <row r="7" spans="1:19" ht="14">
+    <row r="7" spans="1:19" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -3727,7 +3733,7 @@
       <c r="R7" s="41"/>
       <c r="S7" s="38"/>
     </row>
-    <row r="8" spans="1:19" ht="22" customHeight="1">
+    <row r="8" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="42"/>
       <c r="B8" s="42"/>
       <c r="C8" s="42"/>
@@ -3750,7 +3756,7 @@
       <c r="R8" s="46"/>
       <c r="S8" s="38"/>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="47"/>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
@@ -3773,7 +3779,7 @@
       <c r="R9" s="51"/>
       <c r="S9" s="47"/>
     </row>
-    <row r="10" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1">
+    <row r="10" spans="1:19" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -3796,7 +3802,7 @@
       <c r="R10" s="51"/>
       <c r="S10" s="47"/>
     </row>
-    <row r="11" spans="1:19" s="1" customFormat="1" ht="13" customHeight="1">
+    <row r="11" spans="1:19" s="1" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="52"/>
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
@@ -3819,7 +3825,7 @@
       <c r="R11" s="51"/>
       <c r="S11" s="47"/>
     </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" ht="17" customHeight="1">
+    <row r="12" spans="1:19" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="47"/>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
@@ -3842,12 +3848,12 @@
       <c r="R12" s="51"/>
       <c r="S12" s="47"/>
     </row>
-    <row r="13" spans="1:19" ht="17" customHeight="1">
-      <c r="A13" s="108" t="s">
+    <row r="13" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="111" t="s">
         <v>312</v>
       </c>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="72" t="s">
         <v>109</v>
       </c>
@@ -3881,7 +3887,7 @@
       <c r="R13" s="39"/>
       <c r="S13" s="38"/>
     </row>
-    <row r="14" spans="1:19" s="13" customFormat="1" ht="26" customHeight="1">
+    <row r="14" spans="1:19" s="13" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -3899,32 +3905,32 @@
       <c r="O14" s="12"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="1:19" s="18" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="104" t="s">
+    <row r="15" spans="1:19" s="18" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="107" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="105"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="106"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="109"/>
       <c r="K15" s="56"/>
-      <c r="L15" s="104" t="s">
+      <c r="L15" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="M15" s="106"/>
+      <c r="M15" s="109"/>
       <c r="N15" s="56"/>
-      <c r="O15" s="104" t="s">
+      <c r="O15" s="107" t="s">
         <v>281</v>
       </c>
-      <c r="P15" s="105"/>
-      <c r="Q15" s="107"/>
-    </row>
-    <row r="16" spans="1:19" s="18" customFormat="1" ht="13" hidden="1" customHeight="1">
+      <c r="P15" s="108"/>
+      <c r="Q15" s="110"/>
+    </row>
+    <row r="16" spans="1:19" s="18" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19" t="s">
         <v>0</v>
       </c>
@@ -3936,7 +3942,7 @@
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
     </row>
-    <row r="17" spans="1:18" s="26" customFormat="1" ht="41" hidden="1" customHeight="1">
+    <row r="17" spans="1:18" s="26" customFormat="1" ht="41" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="21" t="s">
         <v>1</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="27" customFormat="1" ht="19" hidden="1" customHeight="1">
+    <row r="18" spans="1:18" s="27" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="19" t="s">
         <v>5</v>
       </c>
@@ -4000,7 +4006,7 @@
       <c r="K18" s="32"/>
       <c r="O18" s="28"/>
     </row>
-    <row r="19" spans="1:18" s="27" customFormat="1" ht="56" customHeight="1">
+    <row r="19" spans="1:18" s="27" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
         <v>81</v>
       </c>
@@ -4049,7 +4055,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="27" customFormat="1" ht="13" hidden="1" customHeight="1">
+    <row r="20" spans="1:18" s="27" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
         <v>6</v>
       </c>
@@ -4070,17 +4076,17 @@
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
     </row>
-    <row r="21" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+    <row r="21" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="100" t="s">
-        <v>320</v>
-      </c>
-      <c r="B21" s="109" t="s">
+        <v>323</v>
+      </c>
+      <c r="B21" s="104" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="110" t="s">
+      <c r="D21" s="105" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="93" t="s">
@@ -4089,10 +4095,10 @@
       <c r="F21" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="111" t="s">
+      <c r="G21" s="106" t="s">
         <v>307</v>
       </c>
-      <c r="H21" s="110" t="s">
+      <c r="H21" s="105" t="s">
         <v>268</v>
       </c>
       <c r="I21" s="95" t="s">
@@ -4103,7 +4109,7 @@
       </c>
       <c r="K21" s="64"/>
       <c r="L21" s="96" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="M21" s="97" t="s">
         <v>26</v>
@@ -4116,20 +4122,20 @@
         <v>2</v>
       </c>
       <c r="Q21" s="96" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="100" t="s">
-        <v>321</v>
-      </c>
-      <c r="B22" s="109" t="s">
+        <v>324</v>
+      </c>
+      <c r="B22" s="104" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="105" t="s">
         <v>98</v>
       </c>
       <c r="E22" s="93" t="s">
@@ -4138,10 +4144,10 @@
       <c r="F22" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G22" s="111" t="s">
+      <c r="G22" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="H22" s="110" t="s">
+      <c r="H22" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I22" s="95" t="s">
@@ -4158,17 +4164,17 @@
       <c r="P22" s="65"/>
       <c r="Q22" s="96"/>
     </row>
-    <row r="23" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+    <row r="23" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="100" t="s">
-        <v>322</v>
-      </c>
-      <c r="B23" s="109" t="s">
+        <v>325</v>
+      </c>
+      <c r="B23" s="104" t="s">
         <v>93</v>
       </c>
       <c r="C23" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="110" t="s">
+      <c r="D23" s="105" t="s">
         <v>269</v>
       </c>
       <c r="E23" s="93" t="s">
@@ -4177,10 +4183,10 @@
       <c r="F23" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="111" t="s">
-        <v>323</v>
-      </c>
-      <c r="H23" s="110" t="s">
+      <c r="G23" s="106" t="s">
+        <v>320</v>
+      </c>
+      <c r="H23" s="105" t="s">
         <v>266</v>
       </c>
       <c r="I23" s="95" t="s">
@@ -4197,17 +4203,17 @@
       <c r="P23" s="65"/>
       <c r="Q23" s="96"/>
     </row>
-    <row r="24" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+    <row r="24" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="100" t="s">
-        <v>324</v>
-      </c>
-      <c r="B24" s="109" t="s">
+        <v>326</v>
+      </c>
+      <c r="B24" s="104" t="s">
         <v>95</v>
       </c>
       <c r="C24" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="105" t="s">
         <v>273</v>
       </c>
       <c r="E24" s="93" t="s">
@@ -4216,10 +4222,10 @@
       <c r="F24" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="111" t="s">
+      <c r="G24" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="110" t="s">
+      <c r="H24" s="105" t="s">
         <v>267</v>
       </c>
       <c r="I24" s="95" t="s">
@@ -4236,17 +4242,17 @@
       <c r="P24" s="65"/>
       <c r="Q24" s="96"/>
     </row>
-    <row r="25" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+    <row r="25" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="100" t="s">
-        <v>325</v>
-      </c>
-      <c r="B25" s="109" t="s">
+        <v>327</v>
+      </c>
+      <c r="B25" s="104" t="s">
         <v>96</v>
       </c>
       <c r="C25" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="110" t="s">
+      <c r="D25" s="105" t="s">
         <v>272</v>
       </c>
       <c r="E25" s="93" t="s">
@@ -4255,10 +4261,10 @@
       <c r="F25" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G25" s="111" t="s">
+      <c r="G25" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="110" t="s">
+      <c r="H25" s="105" t="s">
         <v>268</v>
       </c>
       <c r="I25" s="95" t="s">
@@ -4275,17 +4281,17 @@
       <c r="P25" s="65"/>
       <c r="Q25" s="96"/>
     </row>
-    <row r="26" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+    <row r="26" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="100" t="s">
-        <v>326</v>
-      </c>
-      <c r="B26" s="109" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="104" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="110" t="s">
+      <c r="D26" s="105" t="s">
         <v>274</v>
       </c>
       <c r="E26" s="93" t="s">
@@ -4294,10 +4300,10 @@
       <c r="F26" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="111" t="s">
+      <c r="G26" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="110" t="s">
+      <c r="H26" s="105" t="s">
         <v>264</v>
       </c>
       <c r="I26" s="95" t="s">
@@ -4314,17 +4320,17 @@
       <c r="P26" s="65"/>
       <c r="Q26" s="96"/>
     </row>
-    <row r="27" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1">
+    <row r="27" spans="1:18" s="66" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="100" t="s">
-        <v>327</v>
-      </c>
-      <c r="B27" s="109" t="s">
+        <v>329</v>
+      </c>
+      <c r="B27" s="104" t="s">
         <v>94</v>
       </c>
       <c r="C27" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="110" t="s">
+      <c r="D27" s="105" t="s">
         <v>275</v>
       </c>
       <c r="E27" s="93" t="s">
@@ -4333,10 +4339,10 @@
       <c r="F27" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="111" t="s">
+      <c r="G27" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="110" t="s">
+      <c r="H27" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I27" s="95" t="s">
@@ -4353,17 +4359,17 @@
       <c r="P27" s="36"/>
       <c r="Q27" s="98"/>
     </row>
-    <row r="28" spans="1:18" s="66" customFormat="1" ht="11" customHeight="1">
+    <row r="28" spans="1:18" s="66" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="100" t="s">
-        <v>328</v>
-      </c>
-      <c r="B28" s="109" t="s">
+        <v>330</v>
+      </c>
+      <c r="B28" s="104" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="110" t="s">
+      <c r="D28" s="105" t="s">
         <v>100</v>
       </c>
       <c r="E28" s="93" t="s">
@@ -4372,10 +4378,10 @@
       <c r="F28" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="111" t="s">
+      <c r="G28" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="110" t="s">
+      <c r="H28" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I28" s="95" t="s">
@@ -4392,17 +4398,17 @@
       <c r="P28" s="36"/>
       <c r="Q28" s="98"/>
     </row>
-    <row r="29" spans="1:18" s="11" customFormat="1" ht="11" customHeight="1">
+    <row r="29" spans="1:18" s="11" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="100" t="s">
-        <v>329</v>
-      </c>
-      <c r="B29" s="109" t="s">
+        <v>331</v>
+      </c>
+      <c r="B29" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="110" t="s">
+      <c r="D29" s="105" t="s">
         <v>270</v>
       </c>
       <c r="E29" s="93" t="s">
@@ -4411,10 +4417,10 @@
       <c r="F29" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="111" t="s">
+      <c r="G29" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="110" t="s">
+      <c r="H29" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I29" s="95" t="s">
@@ -4432,17 +4438,17 @@
       <c r="Q29" s="96"/>
       <c r="R29" s="66"/>
     </row>
-    <row r="30" spans="1:18" s="11" customFormat="1" ht="12">
+    <row r="30" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="100" t="s">
-        <v>330</v>
-      </c>
-      <c r="B30" s="109" t="s">
+        <v>332</v>
+      </c>
+      <c r="B30" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C30" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="110" t="s">
+      <c r="D30" s="105" t="s">
         <v>101</v>
       </c>
       <c r="E30" s="93" t="s">
@@ -4451,10 +4457,10 @@
       <c r="F30" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="111" t="s">
+      <c r="G30" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H30" s="110" t="s">
+      <c r="H30" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I30" s="95" t="s">
@@ -4472,17 +4478,17 @@
       <c r="Q30" s="96"/>
       <c r="R30" s="66"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="100" t="s">
-        <v>331</v>
-      </c>
-      <c r="B31" s="109" t="s">
+        <v>333</v>
+      </c>
+      <c r="B31" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="110" t="s">
+      <c r="D31" s="105" t="s">
         <v>271</v>
       </c>
       <c r="E31" s="93" t="s">
@@ -4491,10 +4497,10 @@
       <c r="F31" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G31" s="111" t="s">
+      <c r="G31" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="110" t="s">
+      <c r="H31" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I31" s="95" t="s">
@@ -4512,17 +4518,17 @@
       <c r="Q31" s="96"/>
       <c r="R31" s="66"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="100" t="s">
-        <v>332</v>
-      </c>
-      <c r="B32" s="109" t="s">
+        <v>334</v>
+      </c>
+      <c r="B32" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C32" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="110" t="s">
+      <c r="D32" s="105" t="s">
         <v>276</v>
       </c>
       <c r="E32" s="93" t="s">
@@ -4531,10 +4537,10 @@
       <c r="F32" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G32" s="111" t="s">
+      <c r="G32" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="110" t="s">
+      <c r="H32" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I32" s="95" t="s">
@@ -4552,17 +4558,17 @@
       <c r="Q32" s="96"/>
       <c r="R32" s="66"/>
     </row>
-    <row r="33" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="33" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="100" t="s">
-        <v>333</v>
-      </c>
-      <c r="B33" s="109" t="s">
+        <v>335</v>
+      </c>
+      <c r="B33" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C33" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="110" t="s">
+      <c r="D33" s="105" t="s">
         <v>103</v>
       </c>
       <c r="E33" s="93" t="s">
@@ -4571,10 +4577,10 @@
       <c r="F33" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="111" t="s">
+      <c r="G33" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="110" t="s">
+      <c r="H33" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I33" s="95" t="s">
@@ -4592,17 +4598,17 @@
       <c r="Q33" s="96"/>
       <c r="R33" s="66"/>
     </row>
-    <row r="34" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="34" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="100" t="s">
-        <v>334</v>
-      </c>
-      <c r="B34" s="109" t="s">
+        <v>336</v>
+      </c>
+      <c r="B34" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C34" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="110" t="s">
+      <c r="D34" s="105" t="s">
         <v>102</v>
       </c>
       <c r="E34" s="93" t="s">
@@ -4611,10 +4617,10 @@
       <c r="F34" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="111" t="s">
+      <c r="G34" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H34" s="110" t="s">
+      <c r="H34" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I34" s="95" t="s">
@@ -4632,17 +4638,17 @@
       <c r="Q34" s="96"/>
       <c r="R34" s="66"/>
     </row>
-    <row r="35" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="35" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="100" t="s">
-        <v>335</v>
-      </c>
-      <c r="B35" s="109" t="s">
+        <v>337</v>
+      </c>
+      <c r="B35" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="110" t="s">
+      <c r="D35" s="105" t="s">
         <v>202</v>
       </c>
       <c r="E35" s="93" t="s">
@@ -4651,10 +4657,10 @@
       <c r="F35" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="111" t="s">
+      <c r="G35" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H35" s="110" t="s">
+      <c r="H35" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I35" s="95" t="s">
@@ -4672,17 +4678,17 @@
       <c r="Q35" s="98"/>
       <c r="R35" s="66"/>
     </row>
-    <row r="36" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="36" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="100" t="s">
-        <v>336</v>
-      </c>
-      <c r="B36" s="109" t="s">
+        <v>338</v>
+      </c>
+      <c r="B36" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C36" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="110" t="s">
+      <c r="D36" s="105" t="s">
         <v>105</v>
       </c>
       <c r="E36" s="93" t="s">
@@ -4691,10 +4697,10 @@
       <c r="F36" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="111" t="s">
+      <c r="G36" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="110" t="s">
+      <c r="H36" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I36" s="95" t="s">
@@ -4712,17 +4718,17 @@
       <c r="Q36" s="98"/>
       <c r="R36" s="66"/>
     </row>
-    <row r="37" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="37" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A37" s="100" t="s">
-        <v>337</v>
-      </c>
-      <c r="B37" s="109" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C37" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="110" t="s">
+      <c r="D37" s="105" t="s">
         <v>104</v>
       </c>
       <c r="E37" s="93" t="s">
@@ -4731,10 +4737,10 @@
       <c r="F37" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="111" t="s">
+      <c r="G37" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="110" t="s">
+      <c r="H37" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I37" s="95" t="s">
@@ -4752,17 +4758,17 @@
       <c r="Q37" s="96"/>
       <c r="R37" s="66"/>
     </row>
-    <row r="38" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="38" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="100" t="s">
-        <v>338</v>
-      </c>
-      <c r="B38" s="109" t="s">
+        <v>340</v>
+      </c>
+      <c r="B38" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="110" t="s">
+      <c r="D38" s="105" t="s">
         <v>277</v>
       </c>
       <c r="E38" s="93" t="s">
@@ -4771,10 +4777,10 @@
       <c r="F38" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="111" t="s">
+      <c r="G38" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="110" t="s">
+      <c r="H38" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I38" s="95" t="s">
@@ -4792,17 +4798,17 @@
       <c r="Q38" s="96"/>
       <c r="R38" s="66"/>
     </row>
-    <row r="39" spans="1:18" s="6" customFormat="1" ht="12">
+    <row r="39" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="100" t="s">
-        <v>339</v>
-      </c>
-      <c r="B39" s="109" t="s">
+        <v>341</v>
+      </c>
+      <c r="B39" s="104" t="s">
         <v>75</v>
       </c>
       <c r="C39" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="110" t="s">
+      <c r="D39" s="105" t="s">
         <v>304</v>
       </c>
       <c r="E39" s="93" t="s">
@@ -4811,10 +4817,10 @@
       <c r="F39" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="111" t="s">
+      <c r="G39" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="110" t="s">
+      <c r="H39" s="105" t="s">
         <v>265</v>
       </c>
       <c r="I39" s="95" t="s">
@@ -4832,7 +4838,7 @@
       <c r="Q39" s="96"/>
       <c r="R39" s="66"/>
     </row>
-    <row r="40" spans="1:18" s="6" customFormat="1" ht="11">
+    <row r="40" spans="1:18" s="6" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="A40" s="100"/>
       <c r="B40" s="95"/>
       <c r="C40" s="95"/>
@@ -4852,7 +4858,7 @@
       <c r="Q40" s="96"/>
       <c r="R40" s="66"/>
     </row>
-    <row r="41" spans="1:18" s="6" customFormat="1" ht="11">
+    <row r="41" spans="1:18" s="6" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="A41" s="100"/>
       <c r="B41" s="95"/>
       <c r="C41" s="95"/>
@@ -4872,7 +4878,7 @@
       <c r="Q41" s="96"/>
       <c r="R41" s="66"/>
     </row>
-    <row r="42" spans="1:18" s="5" customFormat="1">
+    <row r="42" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A42" s="100"/>
       <c r="B42" s="95"/>
       <c r="C42" s="95"/>
@@ -4892,7 +4898,7 @@
       <c r="Q42" s="96"/>
       <c r="R42" s="66"/>
     </row>
-    <row r="43" spans="1:18" s="5" customFormat="1">
+    <row r="43" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="101"/>
       <c r="B43" s="102"/>
       <c r="C43" s="102"/>
@@ -4912,7 +4918,7 @@
       <c r="Q43" s="98"/>
       <c r="R43" s="66"/>
     </row>
-    <row r="44" spans="1:18" s="5" customFormat="1">
+    <row r="44" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A44" s="101"/>
       <c r="B44" s="102"/>
       <c r="C44" s="102"/>
@@ -4932,7 +4938,7 @@
       <c r="Q44" s="98"/>
       <c r="R44" s="66"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="100"/>
       <c r="B45" s="95"/>
       <c r="C45" s="95"/>
@@ -4952,7 +4958,7 @@
       <c r="Q45" s="96"/>
       <c r="R45" s="66"/>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="100"/>
       <c r="B46" s="95"/>
       <c r="C46" s="95"/>
@@ -4972,7 +4978,7 @@
       <c r="Q46" s="96"/>
       <c r="R46" s="66"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="100"/>
       <c r="B47" s="95"/>
       <c r="C47" s="95"/>
@@ -4992,7 +4998,7 @@
       <c r="Q47" s="96"/>
       <c r="R47" s="66"/>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A48" s="100"/>
       <c r="B48" s="95"/>
       <c r="C48" s="95"/>
@@ -5012,7 +5018,7 @@
       <c r="Q48" s="96"/>
       <c r="R48" s="66"/>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A49" s="100"/>
       <c r="B49" s="95"/>
       <c r="C49" s="95"/>
@@ -5032,7 +5038,7 @@
       <c r="Q49" s="96"/>
       <c r="R49" s="66"/>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="100"/>
       <c r="B50" s="95"/>
       <c r="C50" s="95"/>
@@ -5052,7 +5058,7 @@
       <c r="Q50" s="96"/>
       <c r="R50" s="66"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" s="101"/>
       <c r="B51" s="102"/>
       <c r="C51" s="102"/>
@@ -5072,7 +5078,7 @@
       <c r="Q51" s="98"/>
       <c r="R51" s="66"/>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A52" s="101"/>
       <c r="B52" s="102"/>
       <c r="C52" s="102"/>
@@ -5092,7 +5098,7 @@
       <c r="Q52" s="98"/>
       <c r="R52" s="66"/>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A53" s="100"/>
       <c r="B53" s="95"/>
       <c r="C53" s="95"/>
@@ -5112,7 +5118,7 @@
       <c r="Q53" s="96"/>
       <c r="R53" s="66"/>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A54" s="100"/>
       <c r="B54" s="95"/>
       <c r="C54" s="95"/>
@@ -5132,7 +5138,7 @@
       <c r="Q54" s="96"/>
       <c r="R54" s="66"/>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A55" s="100"/>
       <c r="B55" s="95"/>
       <c r="C55" s="95"/>
@@ -5152,7 +5158,7 @@
       <c r="Q55" s="96"/>
       <c r="R55" s="66"/>
     </row>
-    <row r="56" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="56" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="100"/>
       <c r="B56" s="95"/>
       <c r="C56" s="95"/>
@@ -5172,7 +5178,7 @@
       <c r="Q56" s="96"/>
       <c r="R56" s="66"/>
     </row>
-    <row r="57" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="57" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="100"/>
       <c r="B57" s="95"/>
       <c r="C57" s="95"/>
@@ -5192,7 +5198,7 @@
       <c r="Q57" s="96"/>
       <c r="R57" s="66"/>
     </row>
-    <row r="58" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="58" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="100"/>
       <c r="B58" s="95"/>
       <c r="C58" s="95"/>
@@ -5212,7 +5218,7 @@
       <c r="Q58" s="96"/>
       <c r="R58" s="66"/>
     </row>
-    <row r="59" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="59" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="101"/>
       <c r="B59" s="102"/>
       <c r="C59" s="102"/>
@@ -5232,7 +5238,7 @@
       <c r="Q59" s="98"/>
       <c r="R59" s="66"/>
     </row>
-    <row r="60" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="60" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="101"/>
       <c r="B60" s="102"/>
       <c r="C60" s="102"/>
@@ -5252,7 +5258,7 @@
       <c r="Q60" s="98"/>
       <c r="R60" s="66"/>
     </row>
-    <row r="61" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="61" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="100"/>
       <c r="B61" s="95"/>
       <c r="C61" s="95"/>
@@ -5272,7 +5278,7 @@
       <c r="Q61" s="96"/>
       <c r="R61" s="66"/>
     </row>
-    <row r="62" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="62" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="100"/>
       <c r="B62" s="95"/>
       <c r="C62" s="95"/>
@@ -5292,7 +5298,7 @@
       <c r="Q62" s="96"/>
       <c r="R62" s="66"/>
     </row>
-    <row r="63" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="63" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="100"/>
       <c r="B63" s="95"/>
       <c r="C63" s="95"/>
@@ -5312,7 +5318,7 @@
       <c r="Q63" s="96"/>
       <c r="R63" s="66"/>
     </row>
-    <row r="64" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="64" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="100"/>
       <c r="B64" s="95"/>
       <c r="C64" s="95"/>
@@ -5332,7 +5338,7 @@
       <c r="Q64" s="96"/>
       <c r="R64" s="66"/>
     </row>
-    <row r="65" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="65" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="100"/>
       <c r="B65" s="95"/>
       <c r="C65" s="95"/>
@@ -5352,7 +5358,7 @@
       <c r="Q65" s="96"/>
       <c r="R65" s="66"/>
     </row>
-    <row r="66" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="66" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="100"/>
       <c r="B66" s="95"/>
       <c r="C66" s="95"/>
@@ -5372,7 +5378,7 @@
       <c r="Q66" s="96"/>
       <c r="R66" s="66"/>
     </row>
-    <row r="67" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="67" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="101"/>
       <c r="B67" s="102"/>
       <c r="C67" s="102"/>
@@ -5392,7 +5398,7 @@
       <c r="Q67" s="98"/>
       <c r="R67" s="66"/>
     </row>
-    <row r="68" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1">
+    <row r="68" spans="1:18" s="4" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="101"/>
       <c r="B68" s="102"/>
       <c r="C68" s="102"/>
@@ -5412,7 +5418,7 @@
       <c r="Q68" s="98"/>
       <c r="R68" s="66"/>
     </row>
-    <row r="69" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1">
+    <row r="69" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="100"/>
       <c r="B69" s="95"/>
       <c r="C69" s="95"/>
@@ -5432,7 +5438,7 @@
       <c r="Q69" s="96"/>
       <c r="R69" s="66"/>
     </row>
-    <row r="70" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1">
+    <row r="70" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="100"/>
       <c r="B70" s="95"/>
       <c r="C70" s="95"/>
@@ -5452,7 +5458,7 @@
       <c r="Q70" s="96"/>
       <c r="R70" s="66"/>
     </row>
-    <row r="71" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1">
+    <row r="71" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="100"/>
       <c r="B71" s="95"/>
       <c r="C71" s="95"/>
@@ -5472,7 +5478,7 @@
       <c r="Q71" s="96"/>
       <c r="R71" s="66"/>
     </row>
-    <row r="72" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1">
+    <row r="72" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="100"/>
       <c r="B72" s="95"/>
       <c r="C72" s="95"/>
@@ -5492,7 +5498,7 @@
       <c r="Q72" s="96"/>
       <c r="R72" s="66"/>
     </row>
-    <row r="73" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1">
+    <row r="73" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="100"/>
       <c r="B73" s="95"/>
       <c r="C73" s="95"/>
@@ -5512,7 +5518,7 @@
       <c r="Q73" s="96"/>
       <c r="R73" s="66"/>
     </row>
-    <row r="74" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1">
+    <row r="74" spans="1:18" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="100"/>
       <c r="B74" s="95"/>
       <c r="C74" s="95"/>
@@ -5532,7 +5538,7 @@
       <c r="Q74" s="96"/>
       <c r="R74" s="66"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A75" s="101"/>
       <c r="B75" s="102"/>
       <c r="C75" s="102"/>
@@ -5552,7 +5558,7 @@
       <c r="Q75" s="98"/>
       <c r="R75" s="66"/>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A76" s="101"/>
       <c r="B76" s="102"/>
       <c r="C76" s="102"/>
@@ -5572,7 +5578,7 @@
       <c r="Q76" s="98"/>
       <c r="R76" s="66"/>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A77" s="100"/>
       <c r="B77" s="95"/>
       <c r="C77" s="95"/>
@@ -5592,7 +5598,7 @@
       <c r="Q77" s="96"/>
       <c r="R77" s="66"/>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A78" s="100"/>
       <c r="B78" s="95"/>
       <c r="C78" s="95"/>
@@ -5612,7 +5618,7 @@
       <c r="Q78" s="96"/>
       <c r="R78" s="66"/>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A79" s="100"/>
       <c r="B79" s="95"/>
       <c r="C79" s="95"/>
@@ -5632,7 +5638,7 @@
       <c r="Q79" s="96"/>
       <c r="R79" s="66"/>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A80" s="100"/>
       <c r="B80" s="95"/>
       <c r="C80" s="95"/>
@@ -5652,7 +5658,7 @@
       <c r="Q80" s="96"/>
       <c r="R80" s="66"/>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A81" s="100"/>
       <c r="B81" s="95"/>
       <c r="C81" s="95"/>
@@ -5672,7 +5678,7 @@
       <c r="Q81" s="96"/>
       <c r="R81" s="66"/>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A82" s="100"/>
       <c r="B82" s="95"/>
       <c r="C82" s="95"/>
@@ -5692,7 +5698,7 @@
       <c r="Q82" s="96"/>
       <c r="R82" s="66"/>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A83" s="101"/>
       <c r="B83" s="102"/>
       <c r="C83" s="102"/>
@@ -5712,7 +5718,7 @@
       <c r="Q83" s="98"/>
       <c r="R83" s="66"/>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A84" s="101"/>
       <c r="B84" s="102"/>
       <c r="C84" s="102"/>
@@ -5732,7 +5738,7 @@
       <c r="Q84" s="98"/>
       <c r="R84" s="66"/>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A85" s="100"/>
       <c r="B85" s="95"/>
       <c r="C85" s="95"/>
@@ -5752,7 +5758,7 @@
       <c r="Q85" s="96"/>
       <c r="R85" s="66"/>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A86" s="100"/>
       <c r="B86" s="95"/>
       <c r="C86" s="95"/>
@@ -5772,7 +5778,7 @@
       <c r="Q86" s="96"/>
       <c r="R86" s="66"/>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A87" s="100"/>
       <c r="B87" s="95"/>
       <c r="C87" s="95"/>
@@ -5792,7 +5798,7 @@
       <c r="Q87" s="96"/>
       <c r="R87" s="66"/>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A88" s="100"/>
       <c r="B88" s="95"/>
       <c r="C88" s="95"/>
@@ -5812,7 +5818,7 @@
       <c r="Q88" s="96"/>
       <c r="R88" s="66"/>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A89" s="100"/>
       <c r="B89" s="95"/>
       <c r="C89" s="95"/>
@@ -5832,7 +5838,7 @@
       <c r="Q89" s="96"/>
       <c r="R89" s="66"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A90" s="100"/>
       <c r="B90" s="95"/>
       <c r="C90" s="95"/>
@@ -5852,7 +5858,7 @@
       <c r="Q90" s="96"/>
       <c r="R90" s="66"/>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A91" s="101"/>
       <c r="B91" s="102"/>
       <c r="C91" s="102"/>
@@ -5872,7 +5878,7 @@
       <c r="Q91" s="98"/>
       <c r="R91" s="66"/>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A92" s="101"/>
       <c r="B92" s="102"/>
       <c r="C92" s="102"/>
@@ -5892,7 +5898,7 @@
       <c r="Q92" s="98"/>
       <c r="R92" s="66"/>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A93" s="100"/>
       <c r="B93" s="95"/>
       <c r="C93" s="95"/>
@@ -5912,7 +5918,7 @@
       <c r="Q93" s="96"/>
       <c r="R93" s="66"/>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A94" s="100"/>
       <c r="B94" s="95"/>
       <c r="C94" s="95"/>
@@ -5932,7 +5938,7 @@
       <c r="Q94" s="96"/>
       <c r="R94" s="66"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A95" s="100"/>
       <c r="B95" s="95"/>
       <c r="C95" s="95"/>
@@ -5952,7 +5958,7 @@
       <c r="Q95" s="96"/>
       <c r="R95" s="66"/>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A96" s="100"/>
       <c r="B96" s="95"/>
       <c r="C96" s="95"/>
@@ -5972,7 +5978,7 @@
       <c r="Q96" s="96"/>
       <c r="R96" s="66"/>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A97" s="100"/>
       <c r="B97" s="95"/>
       <c r="C97" s="95"/>
@@ -5992,7 +5998,7 @@
       <c r="Q97" s="96"/>
       <c r="R97" s="66"/>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A98" s="100"/>
       <c r="B98" s="95"/>
       <c r="C98" s="95"/>
@@ -6012,7 +6018,7 @@
       <c r="Q98" s="96"/>
       <c r="R98" s="66"/>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A99" s="101"/>
       <c r="B99" s="102"/>
       <c r="C99" s="102"/>
@@ -6032,7 +6038,7 @@
       <c r="Q99" s="98"/>
       <c r="R99" s="66"/>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A100" s="101"/>
       <c r="B100" s="102"/>
       <c r="C100" s="102"/>
@@ -6052,7 +6058,7 @@
       <c r="Q100" s="98"/>
       <c r="R100" s="66"/>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A101" s="100"/>
       <c r="B101" s="95"/>
       <c r="C101" s="95"/>
@@ -6072,7 +6078,7 @@
       <c r="Q101" s="96"/>
       <c r="R101" s="66"/>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A102" s="100"/>
       <c r="B102" s="95"/>
       <c r="C102" s="95"/>
@@ -6092,7 +6098,7 @@
       <c r="Q102" s="96"/>
       <c r="R102" s="66"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A103" s="100"/>
       <c r="B103" s="95"/>
       <c r="C103" s="95"/>
@@ -6112,7 +6118,7 @@
       <c r="Q103" s="96"/>
       <c r="R103" s="66"/>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A104" s="100"/>
       <c r="B104" s="95"/>
       <c r="C104" s="95"/>
@@ -6132,7 +6138,7 @@
       <c r="Q104" s="96"/>
       <c r="R104" s="66"/>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A105" s="100"/>
       <c r="B105" s="95"/>
       <c r="C105" s="95"/>
@@ -6152,7 +6158,7 @@
       <c r="Q105" s="96"/>
       <c r="R105" s="66"/>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A106" s="100"/>
       <c r="B106" s="95"/>
       <c r="C106" s="95"/>
@@ -6172,7 +6178,7 @@
       <c r="Q106" s="96"/>
       <c r="R106" s="66"/>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A107" s="101"/>
       <c r="B107" s="102"/>
       <c r="C107" s="102"/>
@@ -6192,7 +6198,7 @@
       <c r="Q107" s="98"/>
       <c r="R107" s="66"/>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A108" s="101"/>
       <c r="B108" s="102"/>
       <c r="C108" s="102"/>
@@ -6212,7 +6218,7 @@
       <c r="Q108" s="98"/>
       <c r="R108" s="66"/>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A109" s="100"/>
       <c r="B109" s="95"/>
       <c r="C109" s="95"/>
@@ -6232,7 +6238,7 @@
       <c r="Q109" s="96"/>
       <c r="R109" s="66"/>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A110" s="100"/>
       <c r="B110" s="95"/>
       <c r="C110" s="95"/>
@@ -6252,7 +6258,7 @@
       <c r="Q110" s="96"/>
       <c r="R110" s="66"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A111" s="100"/>
       <c r="B111" s="95"/>
       <c r="C111" s="95"/>
@@ -6272,7 +6278,7 @@
       <c r="Q111" s="96"/>
       <c r="R111" s="66"/>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A112" s="100"/>
       <c r="B112" s="95"/>
       <c r="C112" s="95"/>
@@ -6292,7 +6298,7 @@
       <c r="Q112" s="96"/>
       <c r="R112" s="66"/>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A113" s="100"/>
       <c r="B113" s="95"/>
       <c r="C113" s="95"/>
@@ -6312,7 +6318,7 @@
       <c r="Q113" s="96"/>
       <c r="R113" s="66"/>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A114" s="100"/>
       <c r="B114" s="95"/>
       <c r="C114" s="95"/>
@@ -6332,7 +6338,7 @@
       <c r="Q114" s="96"/>
       <c r="R114" s="66"/>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A115" s="101"/>
       <c r="B115" s="102"/>
       <c r="C115" s="102"/>
@@ -6352,7 +6358,7 @@
       <c r="Q115" s="98"/>
       <c r="R115" s="66"/>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A116" s="101"/>
       <c r="B116" s="102"/>
       <c r="C116" s="102"/>
@@ -6372,7 +6378,7 @@
       <c r="Q116" s="98"/>
       <c r="R116" s="66"/>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A117" s="100"/>
       <c r="B117" s="95"/>
       <c r="C117" s="95"/>
@@ -6392,7 +6398,7 @@
       <c r="Q117" s="96"/>
       <c r="R117" s="66"/>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A118" s="100"/>
       <c r="B118" s="95"/>
       <c r="C118" s="95"/>
@@ -6412,7 +6418,7 @@
       <c r="Q118" s="96"/>
       <c r="R118" s="66"/>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A119" s="100"/>
       <c r="B119" s="95"/>
       <c r="C119" s="95"/>
@@ -6432,7 +6438,7 @@
       <c r="Q119" s="96"/>
       <c r="R119" s="66"/>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A120" s="100"/>
       <c r="B120" s="95"/>
       <c r="C120" s="95"/>
@@ -6452,7 +6458,7 @@
       <c r="Q120" s="96"/>
       <c r="R120" s="66"/>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A121" s="100"/>
       <c r="B121" s="95"/>
       <c r="C121" s="95"/>
@@ -6472,7 +6478,7 @@
       <c r="Q121" s="96"/>
       <c r="R121" s="66"/>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A122" s="100"/>
       <c r="B122" s="95"/>
       <c r="C122" s="95"/>
@@ -6492,7 +6498,7 @@
       <c r="Q122" s="96"/>
       <c r="R122" s="66"/>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A123" s="101"/>
       <c r="B123" s="102"/>
       <c r="C123" s="102"/>
@@ -6512,7 +6518,7 @@
       <c r="Q123" s="98"/>
       <c r="R123" s="66"/>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A124" s="101"/>
       <c r="B124" s="102"/>
       <c r="C124" s="102"/>
@@ -6532,7 +6538,7 @@
       <c r="Q124" s="98"/>
       <c r="R124" s="66"/>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A125" s="100"/>
       <c r="B125" s="95"/>
       <c r="C125" s="95"/>
@@ -6552,7 +6558,7 @@
       <c r="Q125" s="96"/>
       <c r="R125" s="66"/>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A126" s="100"/>
       <c r="B126" s="95"/>
       <c r="C126" s="95"/>
@@ -6572,7 +6578,7 @@
       <c r="Q126" s="96"/>
       <c r="R126" s="66"/>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A127" s="100"/>
       <c r="B127" s="95"/>
       <c r="C127" s="95"/>
@@ -6592,7 +6598,7 @@
       <c r="Q127" s="96"/>
       <c r="R127" s="66"/>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A128" s="100"/>
       <c r="B128" s="95"/>
       <c r="C128" s="95"/>
@@ -6612,7 +6618,7 @@
       <c r="Q128" s="96"/>
       <c r="R128" s="66"/>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A129" s="100"/>
       <c r="B129" s="95"/>
       <c r="C129" s="95"/>
@@ -6632,7 +6638,7 @@
       <c r="Q129" s="96"/>
       <c r="R129" s="66"/>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A130" s="100"/>
       <c r="B130" s="95"/>
       <c r="C130" s="95"/>
@@ -6652,7 +6658,7 @@
       <c r="Q130" s="96"/>
       <c r="R130" s="66"/>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A131" s="101"/>
       <c r="B131" s="102"/>
       <c r="C131" s="102"/>
@@ -6672,7 +6678,7 @@
       <c r="Q131" s="98"/>
       <c r="R131" s="66"/>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A132" s="101"/>
       <c r="B132" s="102"/>
       <c r="C132" s="102"/>
@@ -6692,7 +6698,7 @@
       <c r="Q132" s="98"/>
       <c r="R132" s="66"/>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A133" s="100"/>
       <c r="B133" s="95"/>
       <c r="C133" s="95"/>
@@ -6712,7 +6718,7 @@
       <c r="Q133" s="96"/>
       <c r="R133" s="66"/>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A134" s="100"/>
       <c r="B134" s="95"/>
       <c r="C134" s="95"/>
@@ -6732,7 +6738,7 @@
       <c r="Q134" s="96"/>
       <c r="R134" s="66"/>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A135" s="100"/>
       <c r="B135" s="95"/>
       <c r="C135" s="95"/>
@@ -6752,7 +6758,7 @@
       <c r="Q135" s="96"/>
       <c r="R135" s="66"/>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A136" s="100"/>
       <c r="B136" s="95"/>
       <c r="C136" s="95"/>
@@ -6772,7 +6778,7 @@
       <c r="Q136" s="96"/>
       <c r="R136" s="66"/>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A137" s="100"/>
       <c r="B137" s="95"/>
       <c r="C137" s="95"/>
@@ -6792,7 +6798,7 @@
       <c r="Q137" s="96"/>
       <c r="R137" s="66"/>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A138" s="100"/>
       <c r="B138" s="95"/>
       <c r="C138" s="95"/>
@@ -6812,7 +6818,7 @@
       <c r="Q138" s="96"/>
       <c r="R138" s="66"/>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A139" s="101"/>
       <c r="B139" s="102"/>
       <c r="C139" s="102"/>
@@ -6832,7 +6838,7 @@
       <c r="Q139" s="98"/>
       <c r="R139" s="66"/>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A140" s="101"/>
       <c r="B140" s="102"/>
       <c r="C140" s="102"/>
@@ -6852,7 +6858,7 @@
       <c r="Q140" s="98"/>
       <c r="R140" s="66"/>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A141" s="100"/>
       <c r="B141" s="95"/>
       <c r="C141" s="95"/>
@@ -6872,7 +6878,7 @@
       <c r="Q141" s="96"/>
       <c r="R141" s="66"/>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A142" s="100"/>
       <c r="B142" s="95"/>
       <c r="C142" s="95"/>
@@ -6892,7 +6898,7 @@
       <c r="Q142" s="96"/>
       <c r="R142" s="66"/>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A143" s="100"/>
       <c r="B143" s="95"/>
       <c r="C143" s="95"/>
@@ -6912,7 +6918,7 @@
       <c r="Q143" s="96"/>
       <c r="R143" s="66"/>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A144" s="100"/>
       <c r="B144" s="95"/>
       <c r="C144" s="95"/>
@@ -6932,7 +6938,7 @@
       <c r="Q144" s="96"/>
       <c r="R144" s="66"/>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A145" s="100"/>
       <c r="B145" s="95"/>
       <c r="C145" s="95"/>
@@ -6952,7 +6958,7 @@
       <c r="Q145" s="96"/>
       <c r="R145" s="66"/>
     </row>
-    <row r="146" spans="1:18">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A146" s="100"/>
       <c r="B146" s="95"/>
       <c r="C146" s="95"/>
@@ -6972,7 +6978,7 @@
       <c r="Q146" s="96"/>
       <c r="R146" s="66"/>
     </row>
-    <row r="147" spans="1:18">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A147" s="101"/>
       <c r="B147" s="102"/>
       <c r="C147" s="102"/>
@@ -6992,7 +6998,7 @@
       <c r="Q147" s="98"/>
       <c r="R147" s="66"/>
     </row>
-    <row r="148" spans="1:18">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A148" s="101"/>
       <c r="B148" s="102"/>
       <c r="C148" s="102"/>
@@ -7012,7 +7018,7 @@
       <c r="Q148" s="98"/>
       <c r="R148" s="66"/>
     </row>
-    <row r="149" spans="1:18">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A149" s="100"/>
       <c r="B149" s="95"/>
       <c r="C149" s="95"/>
@@ -7032,7 +7038,7 @@
       <c r="Q149" s="96"/>
       <c r="R149" s="66"/>
     </row>
-    <row r="150" spans="1:18" ht="14" hidden="1">
+    <row r="150" spans="1:18" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A150" s="67" t="s">
         <v>7</v>
       </c>
@@ -7049,8 +7055,8 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" display="https://clinical.scilifelab.se"/>
-    <hyperlink ref="A13:C13" r:id="rId2" display="https://clinical.scilifelab.se/"/>
+    <hyperlink ref="A13" r:id="rId1" display="https://clinical.scilifelab.se" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A13:C13" r:id="rId2" display="https://clinical.scilifelab.se/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="1.05" bottom="1.05" header="0.79000000000000015" footer="0.79000000000000015"/>
   <pageSetup paperSize="9" scale="56" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -7061,67 +7067,67 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$E$1:$E$2</xm:f>
           </x14:formula1>
           <xm:sqref>F21:F149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="See www.clinicalgenomics.se/analyser.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="See www.clinicalgenomics.se/analyser." xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$C$1:$C$19</xm:f>
           </x14:formula1>
           <xm:sqref>D21:D149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$D$1:$D$101</xm:f>
           </x14:formula1>
           <xm:sqref>E21:E149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$H$1:$H$2</xm:f>
           </x14:formula1>
           <xm:sqref>I21:I149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>K21:K149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$J$1:$J$96</xm:f>
           </x14:formula1>
           <xm:sqref>M21:N149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$A$1:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>B21:B149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$B$1</xm:f>
           </x14:formula1>
           <xm:sqref>C21:C149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$G$1:$G$5</xm:f>
           </x14:formula1>
           <xm:sqref>H21:H149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$I$1:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>J21:J149</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If ordering a Nextera or KAPA-based application (METNXTR0xx, MELNXTR0xx, METKAPRxxx) the samples can't be in buffer with enzyme-inhibiting agents such as EDTA. Contact Clinical Genomics before submission, https://clinical.scilifelab.se.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If ordering a Nextera or KAPA-based application (METNXTR0xx, MELNXTR0xx, METKAPRxxx) the samples can't be in buffer with enzyme-inhibiting agents such as EDTA. Contact Clinical Genomics before submission, https://clinical.scilifelab.se." xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$F$1:$F$3</xm:f>
           </x14:formula1>
@@ -7137,14 +7143,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
@@ -7154,7 +7160,7 @@
     <col min="11" max="11" width="11.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
@@ -7186,7 +7192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>93</v>
       </c>
@@ -7216,7 +7222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>95</v>
       </c>
@@ -7240,7 +7246,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>96</v>
       </c>
@@ -7258,7 +7264,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>91</v>
       </c>
@@ -7277,7 +7283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>94</v>
       </c>
@@ -7294,7 +7300,7 @@
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>97</v>
       </c>
@@ -7310,7 +7316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>80</v>
       </c>
@@ -7325,7 +7331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
@@ -7340,7 +7346,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
         <v>101</v>
       </c>
@@ -7351,7 +7357,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
         <v>271</v>
       </c>
@@ -7362,7 +7368,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C12" t="s">
         <v>276</v>
       </c>
@@ -7373,7 +7379,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C13" t="s">
         <v>103</v>
       </c>
@@ -7384,7 +7390,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C14" t="s">
         <v>102</v>
       </c>
@@ -7395,7 +7401,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C15" t="s">
         <v>202</v>
       </c>
@@ -7406,7 +7412,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C16" t="s">
         <v>105</v>
       </c>
@@ -7417,7 +7423,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="3:10">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.15">
       <c r="C17" t="s">
         <v>104</v>
       </c>
@@ -7428,7 +7434,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="3:10">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.15">
       <c r="C18" t="s">
         <v>277</v>
       </c>
@@ -7439,7 +7445,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="3:10">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.15">
       <c r="C19" t="s">
         <v>304</v>
       </c>
@@ -7450,7 +7456,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="3:10">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D20" t="s">
         <v>53</v>
       </c>
@@ -7458,7 +7464,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="3:10">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D21" t="s">
         <v>54</v>
       </c>
@@ -7466,7 +7472,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="3:10">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D22" t="s">
         <v>55</v>
       </c>
@@ -7474,7 +7480,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="3:10">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D23" t="s">
         <v>56</v>
       </c>
@@ -7482,7 +7488,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="3:10">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D24" t="s">
         <v>57</v>
       </c>
@@ -7490,7 +7496,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="3:10">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D25" t="s">
         <v>58</v>
       </c>
@@ -7498,7 +7504,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="3:10">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D26" t="s">
         <v>59</v>
       </c>
@@ -7506,7 +7512,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="3:10">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D27" t="s">
         <v>60</v>
       </c>
@@ -7514,7 +7520,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="3:10">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D28" t="s">
         <v>61</v>
       </c>
@@ -7522,7 +7528,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="3:10">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D29" t="s">
         <v>62</v>
       </c>
@@ -7530,7 +7536,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="3:10">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D30" t="s">
         <v>63</v>
       </c>
@@ -7538,7 +7544,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="3:10">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D31" t="s">
         <v>64</v>
       </c>
@@ -7546,7 +7552,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="3:10">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.15">
       <c r="D32" t="s">
         <v>65</v>
       </c>
@@ -7554,7 +7560,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="4:10">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D33" t="s">
         <v>66</v>
       </c>
@@ -7562,7 +7568,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="4:10">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D34" t="s">
         <v>67</v>
       </c>
@@ -7570,7 +7576,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="4:10">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D35" t="s">
         <v>68</v>
       </c>
@@ -7578,7 +7584,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="4:10">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D36" t="s">
         <v>69</v>
       </c>
@@ -7586,7 +7592,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="4:10">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D37" t="s">
         <v>70</v>
       </c>
@@ -7594,7 +7600,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="4:10">
+    <row r="38" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D38" t="s">
         <v>71</v>
       </c>
@@ -7602,7 +7608,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="4:10">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
         <v>72</v>
       </c>
@@ -7610,7 +7616,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="4:10">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D40" t="s">
         <v>73</v>
       </c>
@@ -7618,7 +7624,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="4:10">
+    <row r="41" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D41" t="s">
         <v>74</v>
       </c>
@@ -7626,7 +7632,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="4:10">
+    <row r="42" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D42" t="s">
         <v>203</v>
       </c>
@@ -7634,7 +7640,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="4:10">
+    <row r="43" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D43" t="s">
         <v>204</v>
       </c>
@@ -7642,7 +7648,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="4:10">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D44" t="s">
         <v>205</v>
       </c>
@@ -7650,7 +7656,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="4:10">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D45" t="s">
         <v>206</v>
       </c>
@@ -7658,7 +7664,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="4:10">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D46" t="s">
         <v>207</v>
       </c>
@@ -7666,7 +7672,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="4:10">
+    <row r="47" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D47" t="s">
         <v>208</v>
       </c>
@@ -7674,7 +7680,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="4:10">
+    <row r="48" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D48" t="s">
         <v>209</v>
       </c>
@@ -7682,7 +7688,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="4:10">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D49" t="s">
         <v>210</v>
       </c>
@@ -7690,7 +7696,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="4:10">
+    <row r="50" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D50" t="s">
         <v>211</v>
       </c>
@@ -7698,7 +7704,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="4:10">
+    <row r="51" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D51" t="s">
         <v>212</v>
       </c>
@@ -7706,7 +7712,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="4:10">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D52" t="s">
         <v>213</v>
       </c>
@@ -7714,7 +7720,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="4:10">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D53" t="s">
         <v>214</v>
       </c>
@@ -7722,7 +7728,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="4:10">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D54" t="s">
         <v>215</v>
       </c>
@@ -7730,7 +7736,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="4:10">
+    <row r="55" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D55" t="s">
         <v>216</v>
       </c>
@@ -7738,7 +7744,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="4:10">
+    <row r="56" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D56" t="s">
         <v>217</v>
       </c>
@@ -7746,7 +7752,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="4:10">
+    <row r="57" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D57" t="s">
         <v>218</v>
       </c>
@@ -7754,7 +7760,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="58" spans="4:10">
+    <row r="58" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D58" t="s">
         <v>219</v>
       </c>
@@ -7762,7 +7768,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="4:10">
+    <row r="59" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D59" t="s">
         <v>220</v>
       </c>
@@ -7770,7 +7776,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="4:10">
+    <row r="60" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D60" t="s">
         <v>221</v>
       </c>
@@ -7778,7 +7784,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="4:10">
+    <row r="61" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D61" t="s">
         <v>222</v>
       </c>
@@ -7786,7 +7792,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="4:10">
+    <row r="62" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D62" t="s">
         <v>223</v>
       </c>
@@ -7794,7 +7800,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="63" spans="4:10">
+    <row r="63" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D63" t="s">
         <v>224</v>
       </c>
@@ -7802,7 +7808,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="4:10">
+    <row r="64" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D64" t="s">
         <v>225</v>
       </c>
@@ -7810,7 +7816,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="4:10">
+    <row r="65" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D65" t="s">
         <v>226</v>
       </c>
@@ -7818,7 +7824,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="66" spans="4:10">
+    <row r="66" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D66" t="s">
         <v>227</v>
       </c>
@@ -7826,7 +7832,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="67" spans="4:10">
+    <row r="67" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D67" t="s">
         <v>228</v>
       </c>
@@ -7834,7 +7840,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="4:10">
+    <row r="68" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D68" t="s">
         <v>229</v>
       </c>
@@ -7842,7 +7848,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="4:10">
+    <row r="69" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D69" t="s">
         <v>230</v>
       </c>
@@ -7850,7 +7856,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="70" spans="4:10">
+    <row r="70" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D70" t="s">
         <v>231</v>
       </c>
@@ -7858,7 +7864,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="4:10">
+    <row r="71" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D71" t="s">
         <v>232</v>
       </c>
@@ -7866,7 +7872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="4:10">
+    <row r="72" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D72" t="s">
         <v>233</v>
       </c>
@@ -7874,7 +7880,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="4:10">
+    <row r="73" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D73" t="s">
         <v>234</v>
       </c>
@@ -7882,7 +7888,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="4:10">
+    <row r="74" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D74" t="s">
         <v>235</v>
       </c>
@@ -7890,7 +7896,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="75" spans="4:10">
+    <row r="75" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D75" t="s">
         <v>236</v>
       </c>
@@ -7898,7 +7904,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="76" spans="4:10">
+    <row r="76" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D76" t="s">
         <v>237</v>
       </c>
@@ -7906,7 +7912,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="4:10">
+    <row r="77" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D77" t="s">
         <v>238</v>
       </c>
@@ -7914,7 +7920,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="4:10">
+    <row r="78" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D78" t="s">
         <v>239</v>
       </c>
@@ -7922,7 +7928,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="4:10">
+    <row r="79" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D79" t="s">
         <v>240</v>
       </c>
@@ -7930,7 +7936,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="4:10">
+    <row r="80" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D80" t="s">
         <v>241</v>
       </c>
@@ -7938,7 +7944,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="4:10">
+    <row r="81" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D81" t="s">
         <v>242</v>
       </c>
@@ -7946,7 +7952,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="4:10">
+    <row r="82" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D82" t="s">
         <v>243</v>
       </c>
@@ -7954,7 +7960,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="83" spans="4:10">
+    <row r="83" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D83" t="s">
         <v>244</v>
       </c>
@@ -7962,7 +7968,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="4:10">
+    <row r="84" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D84" t="s">
         <v>245</v>
       </c>
@@ -7970,7 +7976,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="4:10">
+    <row r="85" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D85" t="s">
         <v>246</v>
       </c>
@@ -7978,7 +7984,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="4:10">
+    <row r="86" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D86" t="s">
         <v>247</v>
       </c>
@@ -7986,7 +7992,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="87" spans="4:10">
+    <row r="87" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D87" t="s">
         <v>248</v>
       </c>
@@ -7994,7 +8000,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="4:10">
+    <row r="88" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D88" t="s">
         <v>249</v>
       </c>
@@ -8002,7 +8008,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="89" spans="4:10">
+    <row r="89" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D89" t="s">
         <v>250</v>
       </c>
@@ -8010,7 +8016,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="90" spans="4:10">
+    <row r="90" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D90" t="s">
         <v>251</v>
       </c>
@@ -8018,7 +8024,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="4:10">
+    <row r="91" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D91" t="s">
         <v>252</v>
       </c>
@@ -8026,7 +8032,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="4:10">
+    <row r="92" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D92" t="s">
         <v>253</v>
       </c>
@@ -8034,7 +8040,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="93" spans="4:10">
+    <row r="93" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D93" t="s">
         <v>254</v>
       </c>
@@ -8042,7 +8048,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="94" spans="4:10">
+    <row r="94" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D94" t="s">
         <v>255</v>
       </c>
@@ -8050,7 +8056,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="95" spans="4:10">
+    <row r="95" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D95" t="s">
         <v>256</v>
       </c>
@@ -8058,7 +8064,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="96" spans="4:10">
+    <row r="96" spans="4:10" x14ac:dyDescent="0.15">
       <c r="D96" t="s">
         <v>257</v>
       </c>
@@ -8066,27 +8072,27 @@
         <v>199</v>
       </c>
     </row>
-    <row r="97" spans="4:4">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D97" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="98" spans="4:4">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D98" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="99" spans="4:4">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D99" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="100" spans="4:4">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D100" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="101" spans="4:4">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D101" t="s">
         <v>262</v>
       </c>

</xml_diff>